<commit_message>
J'ai amélioré l'UI et j'ai créer le bouton pour télécharger le fichier excel des planning
</commit_message>
<xml_diff>
--- a/Matrice de polyvalence1.xlsx
+++ b/Matrice de polyvalence1.xlsx
@@ -5903,11 +5903,11 @@
   <dimension ref="A1:AR43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11420,11 +11420,11 @@
   <dimension ref="A1:AR45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AP22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AP1" activeCellId="0" sqref="AP1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="AT39" activeCellId="0" sqref="AT39"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13817,10 +13817,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>0</v>
@@ -13948,13 +13948,13 @@
         <v>154</v>
       </c>
       <c r="B20" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8" t="n">
         <v>4</v>
-      </c>
-      <c r="C20" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>0</v>
@@ -16360,10 +16360,10 @@
         <v>172</v>
       </c>
       <c r="B38" s="8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38" s="8" t="n">
         <v>3</v>

</xml_diff>